<commit_message>
Uploaded latest Gantt Chart and added Test Cases file
</commit_message>
<xml_diff>
--- a/Project Gantt Chart/Project Gantt Chart Rev A.xlsx
+++ b/Project Gantt Chart/Project Gantt Chart Rev A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{90E5F68B-4645-4308-B766-92FD8F1EA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD7FE0C-2E12-4385-8D3F-99F994BA175E}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{90E5F68B-4645-4308-B766-92FD8F1EA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F664B81-F652-4B60-9567-61BD5AB5D7F0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="415" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>ABOUT THIS GANTT CHART</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Update the Simulink Model based on Test Runs</t>
   </si>
   <si>
-    <t>Run the CAN data through the Simulink Model</t>
-  </si>
-  <si>
     <t>Create Project Report Draft</t>
   </si>
   <si>
@@ -204,6 +201,27 @@
   </si>
   <si>
     <t>Model the BPSK Signal Processing Conversion in Simulink</t>
+  </si>
+  <si>
+    <t>Low Risk</t>
+  </si>
+  <si>
+    <t>Run test cases through the completed Simulink Model</t>
+  </si>
+  <si>
+    <t>Create Github Repository</t>
+  </si>
+  <si>
+    <t>Upload Completed Simulink Models</t>
+  </si>
+  <si>
+    <t>Upload PDFs of Milestone Reports (5 Total)</t>
+  </si>
+  <si>
+    <t>Upload Supporting Documentation (Gantt Chart, Diagrams, etc.)</t>
+  </si>
+  <si>
+    <t>Project Github Repository</t>
   </si>
 </sst>
 </file>
@@ -652,7 +670,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -838,6 +856,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -858,13 +880,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1499,9 +1514,13 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G37" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B9:G37" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G42" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B9:G42" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1809,11 +1828,11 @@
     <row r="2" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
       <c r="F2" s="57"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1841,11 +1860,11 @@
     <row r="4" spans="1:13" s="8" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
       <c r="B4" s="52"/>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="52"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1858,11 +1877,11 @@
     <row r="5" spans="1:13" s="8" customFormat="1" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="52"/>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="52"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1962,10 +1981,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BU40"/>
+  <dimension ref="A1:BU45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:G32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1978,10 +1997,10 @@
     <col min="6" max="6" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="63" width="3.5703125" customWidth="1"/>
+    <col min="9" max="44" width="3.5703125" hidden="1" customWidth="1"/>
+    <col min="45" max="63" width="3.5703125" customWidth="1"/>
     <col min="64" max="64" width="3.28515625" customWidth="1"/>
-    <col min="65" max="65" width="2.7109375" customWidth="1"/>
-    <col min="66" max="73" width="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="73" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2089,36 +2108,36 @@
         <v>5</v>
       </c>
       <c r="H4" s="28"/>
-      <c r="I4" s="75" t="s">
+      <c r="I4" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="N4" s="76" t="s">
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="N4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="S4" s="77" t="s">
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="S4" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="X4" s="73" t="s">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="X4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AC4" s="74" t="s">
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="75"/>
+      <c r="AA4" s="75"/>
+      <c r="AC4" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="76"/>
     </row>
     <row r="5" spans="1:73" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
@@ -3213,7 +3232,7 @@
       </c>
     </row>
     <row r="12" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="66" t="s">
         <v>21</v>
       </c>
@@ -3497,7 +3516,7 @@
       </c>
     </row>
     <row r="13" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="66" t="s">
         <v>24</v>
       </c>
@@ -3781,7 +3800,7 @@
       </c>
     </row>
     <row r="14" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="66" t="s">
         <v>25</v>
       </c>
@@ -3792,7 +3811,7 @@
         <v>23</v>
       </c>
       <c r="E14" s="63">
-        <f>AVERAGE(E34:E37)</f>
+        <f>AVERAGE(E39:E42)</f>
         <v>0</v>
       </c>
       <c r="F14" s="64">
@@ -4065,7 +4084,7 @@
       </c>
     </row>
     <row r="15" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
+      <c r="A15" s="71"/>
       <c r="B15" s="66" t="s">
         <v>26</v>
       </c>
@@ -4076,7 +4095,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="63">
-        <f>AVERAGE(E34:E36,E38)</f>
+        <f>AVERAGE(E39:E41,E43)</f>
         <v>0</v>
       </c>
       <c r="F15" s="64">
@@ -4426,7 +4445,7 @@
       <c r="BU16" s="17"/>
     </row>
     <row r="17" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="66" t="s">
         <v>28</v>
       </c>
@@ -4514,7 +4533,7 @@
       <c r="BU17" s="17"/>
     </row>
     <row r="18" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="78"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="66" t="s">
         <v>30</v>
       </c>
@@ -4602,7 +4621,7 @@
       <c r="BU18" s="17"/>
     </row>
     <row r="19" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="66" t="s">
         <v>31</v>
       </c>
@@ -4690,7 +4709,7 @@
       <c r="BU19" s="17"/>
     </row>
     <row r="20" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="61" t="s">
         <v>32</v>
       </c>
@@ -4962,9 +4981,9 @@
       </c>
     </row>
     <row r="21" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="66" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>29</v>
@@ -5245,7 +5264,7 @@
       </c>
     </row>
     <row r="22" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
+      <c r="A22" s="71"/>
       <c r="B22" s="66" t="s">
         <v>34</v>
       </c>
@@ -5527,9 +5546,9 @@
       </c>
     </row>
     <row r="23" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>29</v>
@@ -5810,9 +5829,9 @@
       </c>
     </row>
     <row r="24" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78"/>
+      <c r="A24" s="71"/>
       <c r="B24" s="66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="62" t="s">
         <v>29</v>
@@ -6093,9 +6112,9 @@
       </c>
     </row>
     <row r="25" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
+      <c r="A25" s="71"/>
       <c r="B25" s="66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="62" t="s">
         <v>29</v>
@@ -6111,7 +6130,7 @@
         <v>45377</v>
       </c>
       <c r="G25" s="65">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="17"/>
@@ -6181,7 +6200,7 @@
       <c r="BU25" s="17"/>
     </row>
     <row r="26" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="66" t="s">
         <v>37</v>
       </c>
@@ -6736,25 +6755,25 @@
       </c>
     </row>
     <row r="28" spans="1:73" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="66" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E28" s="63">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F28" s="64">
-        <f>F23+G23</f>
-        <v>45368</v>
+        <f>F25</f>
+        <v>45377</v>
       </c>
       <c r="G28" s="65">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="17" t="str">
@@ -7019,7 +7038,7 @@
       </c>
     </row>
     <row r="29" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="78"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="66" t="s">
         <v>40</v>
       </c>
@@ -7027,14 +7046,14 @@
         <v>29</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E29" s="63">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F29" s="64">
-        <f>F23+G23</f>
-        <v>45368</v>
+        <f>F25</f>
+        <v>45377</v>
       </c>
       <c r="G29" s="65">
         <v>7</v>
@@ -7107,7 +7126,7 @@
       <c r="BU29" s="17"/>
     </row>
     <row r="30" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="78"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="66" t="s">
         <v>41</v>
       </c>
@@ -7121,11 +7140,11 @@
         <v>0</v>
       </c>
       <c r="F30" s="64">
-        <f>F29+G29</f>
-        <v>45375</v>
+        <f>F29+G29/2</f>
+        <v>45380.5</v>
       </c>
       <c r="G30" s="65">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="17"/>
@@ -7195,9 +7214,9 @@
       <c r="BU30" s="17"/>
     </row>
     <row r="31" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
+      <c r="A31" s="71"/>
       <c r="B31" s="66" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C31" s="62" t="s">
         <v>29</v>
@@ -7210,7 +7229,7 @@
       </c>
       <c r="F31" s="64">
         <f>F30+G30</f>
-        <v>45385</v>
+        <v>45387.5</v>
       </c>
       <c r="G31" s="65">
         <v>1</v>
@@ -7341,7 +7360,7 @@
         <v/>
       </c>
       <c r="AN31" s="17" t="str">
-        <f t="shared" ref="AN31:BC38" ca="1" si="22">IF(AND($C31="Goal",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),1,""))</f>
+        <f t="shared" ref="AN31:BC43" ca="1" si="22">IF(AND($C31="Goal",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),1,""))</f>
         <v/>
       </c>
       <c r="AO31" s="17" t="str">
@@ -7405,7 +7424,7 @@
         <v/>
       </c>
       <c r="BD31" s="17" t="str">
-        <f t="shared" ref="BD31:BS38" ca="1" si="23">IF(AND($C31="Goal",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),1,""))</f>
+        <f t="shared" ref="BD31:BS43" ca="1" si="23">IF(AND($C31="Goal",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),1,""))</f>
         <v/>
       </c>
       <c r="BE31" s="17" t="str">
@@ -7478,9 +7497,9 @@
       </c>
     </row>
     <row r="32" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="62" t="s">
         <v>29</v>
@@ -7492,11 +7511,11 @@
         <v>0</v>
       </c>
       <c r="F32" s="64">
-        <f>F15-13</f>
-        <v>45398</v>
+        <f>F15-19</f>
+        <v>45392</v>
       </c>
       <c r="G32" s="65">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="17" t="str">
@@ -7564,7 +7583,7 @@
         <v/>
       </c>
       <c r="Y32" s="17" t="str">
-        <f t="shared" ref="Y32:AM38" ca="1" si="24">IF(AND($C32="Goal",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),1,""))</f>
+        <f t="shared" ref="Y32:AM43" ca="1" si="24">IF(AND($C32="Goal",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="Z32" s="17" t="str">
@@ -7763,7 +7782,7 @@
     <row r="33" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="61" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C33" s="62"/>
       <c r="D33" s="62"/>
@@ -7771,554 +7790,163 @@
       <c r="F33" s="64"/>
       <c r="G33" s="65"/>
       <c r="H33" s="19"/>
-      <c r="I33" s="17" t="str">
-        <f t="shared" ref="I33:X38" ca="1" si="25">IF(AND($C33="Goal",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1),2,IF(AND($C33="Milestone",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="J33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X33" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AM33" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AN33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AO33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AP33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AQ33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AR33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AS33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AT33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AU33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AV33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AW33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AX33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AY33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AZ33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BA33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BB33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BC33" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BD33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BG33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BH33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BI33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BJ33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BK33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BL33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BM33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BN33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BO33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BP33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BQ33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BR33" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BS33" s="17" t="str">
-        <f t="shared" ref="BS33:BU38" ca="1" si="26">IF(AND($C33="Goal",BS$7&gt;=$F33,BS$7&lt;=$F33+$G33-1),2,IF(AND($C33="Milestone",BS$7&gt;=$F33,BS$7&lt;=$F33+$G33-1),1,""))</f>
-        <v/>
-      </c>
-      <c r="BT33" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BU33" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+      <c r="AE33" s="17"/>
+      <c r="AF33" s="17"/>
+      <c r="AG33" s="17"/>
+      <c r="AH33" s="17"/>
+      <c r="AI33" s="17"/>
+      <c r="AJ33" s="17"/>
+      <c r="AK33" s="17"/>
+      <c r="AL33" s="17"/>
+      <c r="AM33" s="17"/>
+      <c r="AN33" s="17"/>
+      <c r="AO33" s="17"/>
+      <c r="AP33" s="17"/>
+      <c r="AQ33" s="17"/>
+      <c r="AR33" s="17"/>
+      <c r="AS33" s="17"/>
+      <c r="AT33" s="17"/>
+      <c r="AU33" s="17"/>
+      <c r="AV33" s="17"/>
+      <c r="AW33" s="17"/>
+      <c r="AX33" s="17"/>
+      <c r="AY33" s="17"/>
+      <c r="AZ33" s="17"/>
+      <c r="BA33" s="17"/>
+      <c r="BB33" s="17"/>
+      <c r="BC33" s="17"/>
+      <c r="BD33" s="17"/>
+      <c r="BE33" s="17"/>
+      <c r="BF33" s="17"/>
+      <c r="BG33" s="17"/>
+      <c r="BH33" s="17"/>
+      <c r="BI33" s="17"/>
+      <c r="BJ33" s="17"/>
+      <c r="BK33" s="17"/>
+      <c r="BL33" s="17"/>
+      <c r="BM33" s="17"/>
+      <c r="BN33" s="17"/>
+      <c r="BO33" s="17"/>
+      <c r="BP33" s="17"/>
+      <c r="BQ33" s="17"/>
+      <c r="BR33" s="17"/>
+      <c r="BS33" s="17"/>
+      <c r="BT33" s="17"/>
+      <c r="BU33" s="17"/>
     </row>
     <row r="34" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
+      <c r="A34" s="71"/>
       <c r="B34" s="66" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C34" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="62" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E34" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="64">
-        <f>F31+G31</f>
-        <v>45386</v>
+        <v>45373</v>
       </c>
       <c r="G34" s="65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34" s="19"/>
-      <c r="I34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="J34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X34" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AM34" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AN34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AO34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AP34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AQ34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AR34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AS34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AT34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AU34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AV34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AW34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AX34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AY34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AZ34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BA34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BB34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BC34" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BD34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BG34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BH34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BI34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BJ34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BK34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BL34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BM34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BN34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BO34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BP34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BQ34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BR34" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BS34" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BT34" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BU34" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="17"/>
+      <c r="AH34" s="17"/>
+      <c r="AI34" s="17"/>
+      <c r="AJ34" s="17"/>
+      <c r="AK34" s="17"/>
+      <c r="AL34" s="17"/>
+      <c r="AM34" s="17"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="17"/>
+      <c r="AP34" s="17"/>
+      <c r="AQ34" s="17"/>
+      <c r="AR34" s="17"/>
+      <c r="AS34" s="17"/>
+      <c r="AT34" s="17"/>
+      <c r="AU34" s="17"/>
+      <c r="AV34" s="17"/>
+      <c r="AW34" s="17"/>
+      <c r="AX34" s="17"/>
+      <c r="AY34" s="17"/>
+      <c r="AZ34" s="17"/>
+      <c r="BA34" s="17"/>
+      <c r="BB34" s="17"/>
+      <c r="BC34" s="17"/>
+      <c r="BD34" s="17"/>
+      <c r="BE34" s="17"/>
+      <c r="BF34" s="17"/>
+      <c r="BG34" s="17"/>
+      <c r="BH34" s="17"/>
+      <c r="BI34" s="17"/>
+      <c r="BJ34" s="17"/>
+      <c r="BK34" s="17"/>
+      <c r="BL34" s="17"/>
+      <c r="BM34" s="17"/>
+      <c r="BN34" s="17"/>
+      <c r="BO34" s="17"/>
+      <c r="BP34" s="17"/>
+      <c r="BQ34" s="17"/>
+      <c r="BR34" s="17"/>
+      <c r="BS34" s="17"/>
+      <c r="BT34" s="17"/>
+      <c r="BU34" s="17"/>
     </row>
     <row r="35" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="66" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C35" s="62" t="s">
         <v>29</v>
@@ -8330,561 +7958,171 @@
         <v>0</v>
       </c>
       <c r="F35" s="64">
-        <f>F34+G34</f>
-        <v>45388</v>
+        <f>F39</f>
+        <v>45388.5</v>
       </c>
       <c r="G35" s="65">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H35" s="19"/>
-      <c r="I35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="J35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X35" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AM35" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AN35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AO35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AP35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AQ35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AR35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AS35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AT35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AU35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AV35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AW35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AX35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AY35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AZ35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BA35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BB35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BC35" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BD35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BG35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BH35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BI35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BJ35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BK35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BL35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BM35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BN35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BO35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BP35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BQ35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BR35" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BS35" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BT35" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BU35" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
+      <c r="AD35" s="17"/>
+      <c r="AE35" s="17"/>
+      <c r="AF35" s="17"/>
+      <c r="AG35" s="17"/>
+      <c r="AH35" s="17"/>
+      <c r="AI35" s="17"/>
+      <c r="AJ35" s="17"/>
+      <c r="AK35" s="17"/>
+      <c r="AL35" s="17"/>
+      <c r="AM35" s="17"/>
+      <c r="AN35" s="17"/>
+      <c r="AO35" s="17"/>
+      <c r="AP35" s="17"/>
+      <c r="AQ35" s="17"/>
+      <c r="AR35" s="17"/>
+      <c r="AS35" s="17"/>
+      <c r="AT35" s="17"/>
+      <c r="AU35" s="17"/>
+      <c r="AV35" s="17"/>
+      <c r="AW35" s="17"/>
+      <c r="AX35" s="17"/>
+      <c r="AY35" s="17"/>
+      <c r="AZ35" s="17"/>
+      <c r="BA35" s="17"/>
+      <c r="BB35" s="17"/>
+      <c r="BC35" s="17"/>
+      <c r="BD35" s="17"/>
+      <c r="BE35" s="17"/>
+      <c r="BF35" s="17"/>
+      <c r="BG35" s="17"/>
+      <c r="BH35" s="17"/>
+      <c r="BI35" s="17"/>
+      <c r="BJ35" s="17"/>
+      <c r="BK35" s="17"/>
+      <c r="BL35" s="17"/>
+      <c r="BM35" s="17"/>
+      <c r="BN35" s="17"/>
+      <c r="BO35" s="17"/>
+      <c r="BP35" s="17"/>
+      <c r="BQ35" s="17"/>
+      <c r="BR35" s="17"/>
+      <c r="BS35" s="17"/>
+      <c r="BT35" s="17"/>
+      <c r="BU35" s="17"/>
     </row>
     <row r="36" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78"/>
+      <c r="A36" s="71"/>
       <c r="B36" s="66" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C36" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="67" t="s">
+      <c r="D36" s="62" t="s">
         <v>33</v>
       </c>
       <c r="E36" s="63">
-        <v>0</v>
+        <f>3/5</f>
+        <v>0.6</v>
       </c>
       <c r="F36" s="64">
-        <f>F34+G34</f>
-        <v>45388</v>
+        <v>45380</v>
       </c>
       <c r="G36" s="65">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="H36" s="19"/>
-      <c r="I36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="J36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X36" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AM36" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AN36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AO36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AP36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AQ36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AR36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AS36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AT36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AU36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AV36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AW36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AX36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AY36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AZ36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BA36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BB36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BC36" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BD36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BG36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BH36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BI36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BJ36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BK36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BL36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BM36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BN36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BO36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BP36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BQ36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BR36" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BS36" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BT36" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BU36" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
+      <c r="AD36" s="17"/>
+      <c r="AE36" s="17"/>
+      <c r="AF36" s="17"/>
+      <c r="AG36" s="17"/>
+      <c r="AH36" s="17"/>
+      <c r="AI36" s="17"/>
+      <c r="AJ36" s="17"/>
+      <c r="AK36" s="17"/>
+      <c r="AL36" s="17"/>
+      <c r="AM36" s="17"/>
+      <c r="AN36" s="17"/>
+      <c r="AO36" s="17"/>
+      <c r="AP36" s="17"/>
+      <c r="AQ36" s="17"/>
+      <c r="AR36" s="17"/>
+      <c r="AS36" s="17"/>
+      <c r="AT36" s="17"/>
+      <c r="AU36" s="17"/>
+      <c r="AV36" s="17"/>
+      <c r="AW36" s="17"/>
+      <c r="AX36" s="17"/>
+      <c r="AY36" s="17"/>
+      <c r="AZ36" s="17"/>
+      <c r="BA36" s="17"/>
+      <c r="BB36" s="17"/>
+      <c r="BC36" s="17"/>
+      <c r="BD36" s="17"/>
+      <c r="BE36" s="17"/>
+      <c r="BF36" s="17"/>
+      <c r="BG36" s="17"/>
+      <c r="BH36" s="17"/>
+      <c r="BI36" s="17"/>
+      <c r="BJ36" s="17"/>
+      <c r="BK36" s="17"/>
+      <c r="BL36" s="17"/>
+      <c r="BM36" s="17"/>
+      <c r="BN36" s="17"/>
+      <c r="BO36" s="17"/>
+      <c r="BP36" s="17"/>
+      <c r="BQ36" s="17"/>
+      <c r="BR36" s="17"/>
+      <c r="BS36" s="17"/>
+      <c r="BT36" s="17"/>
+      <c r="BU36" s="17"/>
     </row>
-    <row r="37" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="78"/>
+    <row r="37" spans="1:73" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A37" s="71"/>
       <c r="B37" s="66" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C37" s="62" t="s">
         <v>29</v>
@@ -8893,301 +8131,95 @@
         <v>23</v>
       </c>
       <c r="E37" s="63">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F37" s="64">
-        <f>F36+G36</f>
-        <v>45391</v>
+        <f>F36</f>
+        <v>45380</v>
       </c>
       <c r="G37" s="65">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="H37" s="19"/>
-      <c r="I37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="J37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="K37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="L37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="M37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="N37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="O37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="P37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Q37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="R37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="S37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="T37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="U37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="V37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="W37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="X37" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
-      </c>
-      <c r="Y37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="Z37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AA37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AB37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AC37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AD37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AE37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AF37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AG37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AH37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AI37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AJ37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AK37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AL37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AM37" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v/>
-      </c>
-      <c r="AN37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AO37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AP37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AQ37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AR37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AS37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AT37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AU37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AV37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AW37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AX37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AY37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="AZ37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BA37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BB37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BC37" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v/>
-      </c>
-      <c r="BD37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BE37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BF37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BG37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BH37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BI37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BJ37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BK37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BL37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BM37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BN37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BO37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BP37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BQ37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BR37" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
-        <v/>
-      </c>
-      <c r="BS37" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BT37" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
-      <c r="BU37" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
-        <v/>
-      </c>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="17"/>
+      <c r="AB37" s="17"/>
+      <c r="AC37" s="17"/>
+      <c r="AD37" s="17"/>
+      <c r="AE37" s="17"/>
+      <c r="AF37" s="17"/>
+      <c r="AG37" s="17"/>
+      <c r="AH37" s="17"/>
+      <c r="AI37" s="17"/>
+      <c r="AJ37" s="17"/>
+      <c r="AK37" s="17"/>
+      <c r="AL37" s="17"/>
+      <c r="AM37" s="17"/>
+      <c r="AN37" s="17"/>
+      <c r="AO37" s="17"/>
+      <c r="AP37" s="17"/>
+      <c r="AQ37" s="17"/>
+      <c r="AR37" s="17"/>
+      <c r="AS37" s="17"/>
+      <c r="AT37" s="17"/>
+      <c r="AU37" s="17"/>
+      <c r="AV37" s="17"/>
+      <c r="AW37" s="17"/>
+      <c r="AX37" s="17"/>
+      <c r="AY37" s="17"/>
+      <c r="AZ37" s="17"/>
+      <c r="BA37" s="17"/>
+      <c r="BB37" s="17"/>
+      <c r="BC37" s="17"/>
+      <c r="BD37" s="17"/>
+      <c r="BE37" s="17"/>
+      <c r="BF37" s="17"/>
+      <c r="BG37" s="17"/>
+      <c r="BH37" s="17"/>
+      <c r="BI37" s="17"/>
+      <c r="BJ37" s="17"/>
+      <c r="BK37" s="17"/>
+      <c r="BL37" s="17"/>
+      <c r="BM37" s="17"/>
+      <c r="BN37" s="17"/>
+      <c r="BO37" s="17"/>
+      <c r="BP37" s="17"/>
+      <c r="BQ37" s="17"/>
+      <c r="BR37" s="17"/>
+      <c r="BS37" s="17"/>
+      <c r="BT37" s="17"/>
+      <c r="BU37" s="17"/>
     </row>
     <row r="38" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="78"/>
-      <c r="B38" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="63">
-        <v>0</v>
-      </c>
-      <c r="F38" s="64">
-        <f>F36+G36</f>
-        <v>45391</v>
-      </c>
-      <c r="G38" s="65">
-        <v>7</v>
-      </c>
+      <c r="A38" s="9"/>
+      <c r="B38" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="19"/>
       <c r="I38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ref="I38:X43" ca="1" si="25">IF(AND($C38="Goal",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="J38" s="17" t="str">
@@ -9435,7 +8467,7 @@
         <v/>
       </c>
       <c r="BS38" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ref="BS38:BU43" ca="1" si="26">IF(AND($C38="Goal",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BT38" s="17" t="str">
@@ -9447,13 +8479,1428 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:73" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="3"/>
+    <row r="39" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="71"/>
+      <c r="B39" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="63">
+        <v>0</v>
+      </c>
+      <c r="F39" s="64">
+        <f>F31+G31</f>
+        <v>45388.5</v>
+      </c>
+      <c r="G39" s="65">
+        <v>2</v>
+      </c>
+      <c r="H39" s="19"/>
+      <c r="I39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="J39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="K39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="L39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="M39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="N39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="O39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="P39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Q39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="R39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="S39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="T39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="U39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="V39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="W39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="X39" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Y39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="Z39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AA39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AB39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AC39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AD39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AE39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AF39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AG39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AH39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AI39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AJ39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AK39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AL39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AM39" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AN39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AO39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AP39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AQ39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AR39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AS39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AT39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AU39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AV39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AW39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AX39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AY39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AZ39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BA39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BC39" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BD39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BE39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BF39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BG39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BH39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BI39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BJ39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BK39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BL39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BM39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BN39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BO39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BP39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BQ39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BR39" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BS39" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BT39" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BU39" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
     </row>
-    <row r="40" spans="1:73" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="5"/>
+    <row r="40" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="71"/>
+      <c r="B40" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="63">
+        <v>0</v>
+      </c>
+      <c r="F40" s="64">
+        <f>F39+G39</f>
+        <v>45390.5</v>
+      </c>
+      <c r="G40" s="65">
+        <v>2</v>
+      </c>
+      <c r="H40" s="19"/>
+      <c r="I40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="J40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="L40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="M40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="N40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="O40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="P40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Q40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="R40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="S40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="T40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="U40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="V40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="W40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="X40" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Y40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="Z40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AA40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AB40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AC40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AD40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AE40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AF40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AG40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AH40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AI40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AJ40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AK40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AL40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AM40" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AN40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AO40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AP40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AQ40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AR40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AS40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AT40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AU40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AV40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AW40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AX40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AY40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AZ40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BA40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BC40" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BD40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BE40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BF40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BG40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BH40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BI40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BJ40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BK40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BL40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BM40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BN40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BO40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BP40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BQ40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BR40" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BS40" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BT40" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BU40" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="71"/>
+      <c r="B41" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="63">
+        <v>0</v>
+      </c>
+      <c r="F41" s="64">
+        <f>F39+G39</f>
+        <v>45390.5</v>
+      </c>
+      <c r="G41" s="65">
+        <v>3</v>
+      </c>
+      <c r="H41" s="19"/>
+      <c r="I41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="J41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="K41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="L41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="M41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="N41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="O41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="P41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Q41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="R41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="S41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="T41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="U41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="V41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="W41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="X41" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Y41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="Z41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AA41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AB41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AC41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AD41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AE41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AF41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AG41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AH41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AI41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AJ41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AK41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AL41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AM41" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AN41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AO41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AP41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AQ41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AR41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AS41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AT41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AU41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AV41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AW41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AX41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AY41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AZ41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BA41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BC41" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BD41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BE41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BF41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BG41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BH41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BI41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BJ41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BK41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BL41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BM41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BN41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BO41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BP41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BQ41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BR41" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BS41" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BT41" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BU41" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="71"/>
+      <c r="B42" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="63">
+        <v>0</v>
+      </c>
+      <c r="F42" s="64">
+        <f>F41+G41</f>
+        <v>45393.5</v>
+      </c>
+      <c r="G42" s="65">
+        <v>5</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="J42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="K42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="L42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="M42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="N42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="O42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="P42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Q42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="R42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="S42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="T42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="U42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="V42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="W42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="X42" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Y42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="Z42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AA42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AB42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AC42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AD42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AE42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AF42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AG42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AH42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AI42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AJ42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AK42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AL42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AM42" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AN42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AO42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AP42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AQ42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AR42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AS42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AT42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AU42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AV42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AW42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AX42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AY42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AZ42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BA42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BC42" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BD42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BE42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BF42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BG42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BH42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BI42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BJ42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BK42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BL42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BM42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BN42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BO42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BP42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BQ42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BR42" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BS42" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BT42" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BU42" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="71"/>
+      <c r="B43" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="63">
+        <v>0</v>
+      </c>
+      <c r="F43" s="64">
+        <f>F42+G42-1</f>
+        <v>45397.5</v>
+      </c>
+      <c r="G43" s="65">
+        <v>15</v>
+      </c>
+      <c r="H43" s="19"/>
+      <c r="I43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="J43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="K43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="L43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="M43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="N43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="O43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="P43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Q43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="R43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="S43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="T43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="U43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="V43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="W43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="X43" s="17" t="str">
+        <f t="shared" ca="1" si="25"/>
+        <v/>
+      </c>
+      <c r="Y43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="Z43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AA43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AB43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AC43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AD43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AE43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AF43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AG43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AH43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AI43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AJ43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AK43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AL43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AM43" s="17" t="str">
+        <f t="shared" ca="1" si="24"/>
+        <v/>
+      </c>
+      <c r="AN43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AO43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AP43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AQ43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AR43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AS43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AT43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AU43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AV43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AW43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AX43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AY43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="AZ43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BA43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BB43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BC43" s="17" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v/>
+      </c>
+      <c r="BD43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BE43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BF43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BG43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BH43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BI43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BJ43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BK43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BL43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BM43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BN43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BO43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BP43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BQ43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BR43" s="17" t="str">
+        <f t="shared" ca="1" si="23"/>
+        <v/>
+      </c>
+      <c r="BS43" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BT43" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+      <c r="BU43" s="17" t="str">
+        <f t="shared" ca="1" si="26"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:73" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="4"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:73" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -9463,7 +9910,7 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E38">
+  <conditionalFormatting sqref="E9:E43">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9482,7 +9929,7 @@
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BT38">
+  <conditionalFormatting sqref="I7:BT43">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
@@ -9492,7 +9939,7 @@
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BU38">
+  <conditionalFormatting sqref="I10:BU43">
     <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
@@ -9514,7 +9961,7 @@
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BU7:BU38">
+  <conditionalFormatting sqref="BU7:BU43">
     <cfRule type="expression" dxfId="0" priority="49">
       <formula>AND(TODAY()&gt;=BU$7,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -9523,7 +9970,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{662A47A0-7258-440E-8D71-BC54CBC9C651}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C38" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C43" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{218D9212-09C8-4DA2-9014-64503951B170}">
@@ -9540,7 +9987,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup scale="38" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="61" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -9561,7 +10008,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E38</xm:sqref>
+          <xm:sqref>E9:E43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="97" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
@@ -9580,7 +10027,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BU38</xm:sqref>
+          <xm:sqref>I10:BU43</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9589,6 +10036,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="81dd9769-e470-4c71-abd0-ce40395fb0d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="97f26d6d-5e45-4b6a-a489-05413f707488" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9597,7 +10055,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100329040CD17E650448811C75D3A86FB19" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4e7394bae465e0dd152f3bf3519e0af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81dd9769-e470-4c71-abd0-ce40395fb0d0" xmlns:ns3="97f26d6d-5e45-4b6a-a489-05413f707488" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f30c7f853ad86ef2df9f5f9817cec86e" ns2:_="" ns3:_="">
     <xsd:import namespace="81dd9769-e470-4c71-abd0-ce40395fb0d0"/>
@@ -9786,18 +10244,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="81dd9769-e470-4c71-abd0-ce40395fb0d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="97f26d6d-5e45-4b6a-a489-05413f707488" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="81dd9769-e470-4c71-abd0-ce40395fb0d0"/>
+    <ds:schemaRef ds:uri="97f26d6d-5e45-4b6a-a489-05413f707488"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -9805,7 +10263,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDC3097-99E4-4C58-971A-CB9D833D16FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9824,17 +10282,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81dd9769-e470-4c71-abd0-ce40395fb0d0"/>
-    <ds:schemaRef ds:uri="97f26d6d-5e45-4b6a-a489-05413f707488"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Updated Gantt Chart for Milestone #3.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart/Project Gantt Chart Rev A.xlsx
+++ b/Project Gantt Chart/Project Gantt Chart Rev A.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{90E5F68B-4645-4308-B766-92FD8F1EA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F664B81-F652-4B60-9567-61BD5AB5D7F0}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="8_{90E5F68B-4645-4308-B766-92FD8F1EA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3D0263E-B64E-4F9F-A52F-04A2C0071F7B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="415" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>Andrew Cline</t>
   </si>
   <si>
-    <t>Model the Transmitter and Receiver in Simulink</t>
-  </si>
-  <si>
     <t>Clifford Gilbert</t>
   </si>
   <si>
@@ -191,18 +188,6 @@
     <t>Develop Project Report Documentation</t>
   </si>
   <si>
-    <t>Create the CAN bus model in Simulink</t>
-  </si>
-  <si>
-    <t>Create the data encryption model in Simulink</t>
-  </si>
-  <si>
-    <t>Create data transfer from integer input to data signal</t>
-  </si>
-  <si>
-    <t>Model the BPSK Signal Processing Conversion in Simulink</t>
-  </si>
-  <si>
     <t>Low Risk</t>
   </si>
   <si>
@@ -222,6 +207,21 @@
   </si>
   <si>
     <t>Project Github Repository</t>
+  </si>
+  <si>
+    <t>Create data transfer from integer to data signal</t>
+  </si>
+  <si>
+    <t>Create the data encryption model</t>
+  </si>
+  <si>
+    <t>Model the BPSK Signal Processing Conversion</t>
+  </si>
+  <si>
+    <t>Model the Transmitter and Receiver</t>
+  </si>
+  <si>
+    <t>Create the CAN bus model</t>
   </si>
 </sst>
 </file>
@@ -896,7 +896,145 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1349,21 +1487,21 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="4" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="30"/>
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="39"/>
+      <tableStyleElement type="firstRowStripe" dxfId="38"/>
+      <tableStyleElement type="secondRowStripe" dxfId="37"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumn" dxfId="23"/>
-      <tableStyleElement type="lastColumn" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="secondRowStripe" dxfId="20"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="36"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="totalRow" dxfId="34"/>
+      <tableStyleElement type="firstColumn" dxfId="33"/>
+      <tableStyleElement type="lastColumn" dxfId="32"/>
+      <tableStyleElement type="firstRowStripe" dxfId="31"/>
+      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="29"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1519,7 +1657,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G42" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G42" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B9:G42" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1529,12 +1667,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="11" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="10" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="21" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="20" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1983,8 +2121,8 @@
   </sheetPr>
   <dimension ref="A1:BU45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3365,7 @@
         <v/>
       </c>
       <c r="BU11" s="17" t="str">
-        <f t="shared" ref="BS11:BU32" ca="1" si="19">IF(AND($C11="Goal",BU$7&gt;=$F11,BU$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",BU$7&gt;=$F11,BU$7&lt;=$F11+$G11-1),1,""))</f>
+        <f t="shared" ref="BS11:BU31" ca="1" si="19">IF(AND($C11="Goal",BU$7&gt;=$F11,BU$7&lt;=$F11+$G11-1),2,IF(AND($C11="Milestone",BU$7&gt;=$F11,BU$7&lt;=$F11+$G11-1),1,""))</f>
         <v/>
       </c>
     </row>
@@ -3539,7 +3677,7 @@
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="17" t="str">
-        <f t="shared" ref="I13:X32" ca="1" si="20">IF(AND($C13="Goal",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Milestone",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
+        <f t="shared" ref="I13:I31" ca="1" si="20">IF(AND($C13="Goal",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),2,IF(AND($C13="Milestone",I$7&gt;=$F13,I$7&lt;=$F13+$G13-1),1,""))</f>
         <v/>
       </c>
       <c r="J13" s="17" t="str">
@@ -4983,13 +5121,13 @@
     <row r="21" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
       <c r="B21" s="66" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="63">
         <v>1</v>
@@ -5266,13 +5404,13 @@
     <row r="22" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="71"/>
       <c r="B22" s="66" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C22" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="63">
         <v>1</v>
@@ -5548,7 +5686,7 @@
     <row r="23" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="71"/>
       <c r="B23" s="66" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>29</v>
@@ -5831,13 +5969,13 @@
     <row r="24" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="71"/>
       <c r="B24" s="66" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C24" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="63">
         <v>1</v>
@@ -6114,13 +6252,13 @@
     <row r="25" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="71"/>
       <c r="B25" s="66" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C25" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="63">
         <v>1</v>
@@ -6202,7 +6340,7 @@
     <row r="26" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="71"/>
       <c r="B26" s="66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="62" t="s">
         <v>29</v>
@@ -6485,7 +6623,7 @@
     <row r="27" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="62"/>
       <c r="D27" s="62"/>
@@ -6757,10 +6895,10 @@
     <row r="28" spans="1:73" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="71"/>
       <c r="B28" s="66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D28" s="62" t="s">
         <v>33</v>
@@ -7040,13 +7178,13 @@
     <row r="29" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="71"/>
       <c r="B29" s="66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E29" s="63">
         <v>0.5</v>
@@ -7056,7 +7194,7 @@
         <v>45377</v>
       </c>
       <c r="G29" s="65">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="17"/>
@@ -7128,7 +7266,7 @@
     <row r="30" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="71"/>
       <c r="B30" s="66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="62" t="s">
         <v>29</v>
@@ -7141,10 +7279,10 @@
       </c>
       <c r="F30" s="64">
         <f>F29+G29/2</f>
-        <v>45380.5</v>
+        <v>45382</v>
       </c>
       <c r="G30" s="65">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="17"/>
@@ -7216,20 +7354,20 @@
     <row r="31" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="71"/>
       <c r="B31" s="66" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C31" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="63">
         <v>0</v>
       </c>
       <c r="F31" s="64">
         <f>F30+G30</f>
-        <v>45387.5</v>
+        <v>45387</v>
       </c>
       <c r="G31" s="65">
         <v>1</v>
@@ -7360,7 +7498,7 @@
         <v/>
       </c>
       <c r="AN31" s="17" t="str">
-        <f t="shared" ref="AN31:BC43" ca="1" si="22">IF(AND($C31="Goal",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),1,""))</f>
+        <f t="shared" ref="AN31" ca="1" si="22">IF(AND($C31="Goal",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",AN$7&gt;=$F31,AN$7&lt;=$F31+$G31-1),1,""))</f>
         <v/>
       </c>
       <c r="AO31" s="17" t="str">
@@ -7424,7 +7562,7 @@
         <v/>
       </c>
       <c r="BD31" s="17" t="str">
-        <f t="shared" ref="BD31:BS43" ca="1" si="23">IF(AND($C31="Goal",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),1,""))</f>
+        <f t="shared" ref="BD31" ca="1" si="23">IF(AND($C31="Goal",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),2,IF(AND($C31="Milestone",BD$7&gt;=$F31,BD$7&lt;=$F31+$G31-1),1,""))</f>
         <v/>
       </c>
       <c r="BE31" s="17" t="str">
@@ -7499,7 +7637,7 @@
     <row r="32" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="71"/>
       <c r="B32" s="66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="62" t="s">
         <v>29</v>
@@ -7519,159 +7657,159 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="J32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",J$7&gt;=$F32,J$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",J$7&gt;=$F32,J$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="K32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",K$7&gt;=$F32,K$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",K$7&gt;=$F32,K$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="L32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",L$7&gt;=$F32,L$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",L$7&gt;=$F32,L$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="M32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",M$7&gt;=$F32,M$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",M$7&gt;=$F32,M$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="N32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",N$7&gt;=$F32,N$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",N$7&gt;=$F32,N$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="O32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",O$7&gt;=$F32,O$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",O$7&gt;=$F32,O$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="P32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",P$7&gt;=$F32,P$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",P$7&gt;=$F32,P$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="Q32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",Q$7&gt;=$F32,Q$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Q$7&gt;=$F32,Q$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="R32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",R$7&gt;=$F32,R$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",R$7&gt;=$F32,R$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="S32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",S$7&gt;=$F32,S$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",S$7&gt;=$F32,S$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="T32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",T$7&gt;=$F32,T$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",T$7&gt;=$F32,T$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="U32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",U$7&gt;=$F32,U$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",U$7&gt;=$F32,U$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="V32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",V$7&gt;=$F32,V$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",V$7&gt;=$F32,V$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="W32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",W$7&gt;=$F32,W$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",W$7&gt;=$F32,W$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="X32" s="17" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f ca="1">IF(AND($C32="Goal",X$7&gt;=$F32,X$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",X$7&gt;=$F32,X$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="Y32" s="17" t="str">
-        <f t="shared" ref="Y32:AM43" ca="1" si="24">IF(AND($C32="Goal",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),1,""))</f>
+        <f ca="1">IF(AND($C32="Goal",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Y$7&gt;=$F32,Y$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="Z32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",Z$7&gt;=$F32,Z$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",Z$7&gt;=$F32,Z$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AA32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AA$7&gt;=$F32,AA$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AA$7&gt;=$F32,AA$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AB32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AB$7&gt;=$F32,AB$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AB$7&gt;=$F32,AB$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AC32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AC$7&gt;=$F32,AC$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AC$7&gt;=$F32,AC$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AD32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AD$7&gt;=$F32,AD$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AD$7&gt;=$F32,AD$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AE32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AE$7&gt;=$F32,AE$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AE$7&gt;=$F32,AE$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AF32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AF$7&gt;=$F32,AF$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AF$7&gt;=$F32,AF$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AG32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AG$7&gt;=$F32,AG$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AG$7&gt;=$F32,AG$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AH32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AH$7&gt;=$F32,AH$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AH$7&gt;=$F32,AH$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AI32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AI$7&gt;=$F32,AI$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AI$7&gt;=$F32,AI$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AJ$7&gt;=$F32,AJ$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AJ$7&gt;=$F32,AJ$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AK32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AK$7&gt;=$F32,AK$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AK$7&gt;=$F32,AK$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AL32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AL$7&gt;=$F32,AL$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AL$7&gt;=$F32,AL$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AM32" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C32="Goal",AM$7&gt;=$F32,AM$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AM$7&gt;=$F32,AM$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AN32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AN$7&gt;=$F32,AN$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AO32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AO$7&gt;=$F32,AO$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AO$7&gt;=$F32,AO$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AP32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AP$7&gt;=$F32,AP$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AP$7&gt;=$F32,AP$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AQ$7&gt;=$F32,AQ$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AQ$7&gt;=$F32,AQ$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AR32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AR$7&gt;=$F32,AR$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AR$7&gt;=$F32,AR$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AS32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AS$7&gt;=$F32,AS$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AS$7&gt;=$F32,AS$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AT32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AT$7&gt;=$F32,AT$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AT$7&gt;=$F32,AT$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AU32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AU$7&gt;=$F32,AU$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AU$7&gt;=$F32,AU$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AV32" s="17" t="str">
@@ -7679,110 +7817,110 @@
         <v/>
       </c>
       <c r="AW32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AW$7&gt;=$F32,AW$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AW$7&gt;=$F32,AW$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AX32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AX$7&gt;=$F32,AX$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AX$7&gt;=$F32,AX$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AY32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AY$7&gt;=$F32,AY$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AY$7&gt;=$F32,AY$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",AZ$7&gt;=$F32,AZ$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",AZ$7&gt;=$F32,AZ$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BA32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",BA$7&gt;=$F32,BA$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BA$7&gt;=$F32,BA$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BB32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",BB$7&gt;=$F32,BB$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BB$7&gt;=$F32,BB$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BC32" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C32="Goal",BC$7&gt;=$F32,BC$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BC$7&gt;=$F32,BC$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BD32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BD$7&gt;=$F32,BD$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BE32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BE$7&gt;=$F32,BE$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BE$7&gt;=$F32,BE$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BF32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BF$7&gt;=$F32,BF$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BF$7&gt;=$F32,BF$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BG32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BG$7&gt;=$F32,BG$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BG$7&gt;=$F32,BG$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BH32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BH$7&gt;=$F32,BH$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BH$7&gt;=$F32,BH$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BI32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BI$7&gt;=$F32,BI$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BI$7&gt;=$F32,BI$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BJ$7&gt;=$F32,BJ$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BJ$7&gt;=$F32,BJ$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BK32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BK$7&gt;=$F32,BK$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BK$7&gt;=$F32,BK$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BL32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BL$7&gt;=$F32,BL$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BL$7&gt;=$F32,BL$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BM32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BM$7&gt;=$F32,BM$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BM$7&gt;=$F32,BM$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BN32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BN$7&gt;=$F32,BN$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BN$7&gt;=$F32,BN$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BO32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BO$7&gt;=$F32,BO$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BO$7&gt;=$F32,BO$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BP32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BP$7&gt;=$F32,BP$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BP$7&gt;=$F32,BP$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BQ$7&gt;=$F32,BQ$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BQ$7&gt;=$F32,BQ$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BR32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BR$7&gt;=$F32,BR$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BR$7&gt;=$F32,BR$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BS32" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C32="Goal",BS$7&gt;=$F32,BS$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BS$7&gt;=$F32,BS$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BT32" s="17" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f ca="1">IF(AND($C32="Goal",BT$7&gt;=$F32,BT$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BT$7&gt;=$F32,BT$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
       <c r="BU32" s="17" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f ca="1">IF(AND($C32="Goal",BU$7&gt;=$F32,BU$7&lt;=$F32+$G32-1),2,IF(AND($C32="Milestone",BU$7&gt;=$F32,BU$7&lt;=$F32+$G32-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="61" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C33" s="62"/>
       <c r="D33" s="62"/>
@@ -7859,13 +7997,13 @@
     <row r="34" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="71"/>
       <c r="B34" s="66" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C34" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" s="63">
         <v>1</v>
@@ -7946,20 +8084,20 @@
     <row r="35" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="71"/>
       <c r="B35" s="66" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C35" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" s="63">
         <v>0</v>
       </c>
       <c r="F35" s="64">
         <f>F39</f>
-        <v>45388.5</v>
+        <v>45388</v>
       </c>
       <c r="G35" s="65">
         <v>14</v>
@@ -8034,7 +8172,7 @@
     <row r="36" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="71"/>
       <c r="B36" s="66" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C36" s="62" t="s">
         <v>29</v>
@@ -8122,7 +8260,7 @@
     <row r="37" spans="1:73" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A37" s="71"/>
       <c r="B37" s="66" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C37" s="62" t="s">
         <v>29</v>
@@ -8131,7 +8269,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="63">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="F37" s="64">
         <f>F36</f>
@@ -8210,7 +8348,7 @@
     <row r="38" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="62"/>
       <c r="D38" s="62"/>
@@ -8219,270 +8357,270 @@
       <c r="G38" s="65"/>
       <c r="H38" s="19"/>
       <c r="I38" s="17" t="str">
-        <f t="shared" ref="I38:X43" ca="1" si="25">IF(AND($C38="Goal",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),1,""))</f>
+        <f ca="1">IF(AND($C38="Goal",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",I$7&gt;=$F38,I$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="J38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",J$7&gt;=$F38,J$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",J$7&gt;=$F38,J$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="K38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",K$7&gt;=$F38,K$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",K$7&gt;=$F38,K$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="L38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",L$7&gt;=$F38,L$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",L$7&gt;=$F38,L$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="M38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",M$7&gt;=$F38,M$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",M$7&gt;=$F38,M$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="N38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",N$7&gt;=$F38,N$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",N$7&gt;=$F38,N$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="O38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",O$7&gt;=$F38,O$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",O$7&gt;=$F38,O$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="P38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",P$7&gt;=$F38,P$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",P$7&gt;=$F38,P$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="Q38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",Q$7&gt;=$F38,Q$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",Q$7&gt;=$F38,Q$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="R38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",R$7&gt;=$F38,R$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",R$7&gt;=$F38,R$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="S38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",S$7&gt;=$F38,S$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",S$7&gt;=$F38,S$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="T38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",T$7&gt;=$F38,T$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",T$7&gt;=$F38,T$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="U38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",U$7&gt;=$F38,U$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",U$7&gt;=$F38,U$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="V38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",V$7&gt;=$F38,V$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",V$7&gt;=$F38,V$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="W38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",W$7&gt;=$F38,W$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",W$7&gt;=$F38,W$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="X38" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C38="Goal",X$7&gt;=$F38,X$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",X$7&gt;=$F38,X$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="Y38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",Y$7&gt;=$F38,Y$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",Y$7&gt;=$F38,Y$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="Z38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",Z$7&gt;=$F38,Z$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",Z$7&gt;=$F38,Z$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AA38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AA$7&gt;=$F38,AA$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AA$7&gt;=$F38,AA$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AB38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AB$7&gt;=$F38,AB$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AB$7&gt;=$F38,AB$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AC38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AC$7&gt;=$F38,AC$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AC$7&gt;=$F38,AC$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AD38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AD$7&gt;=$F38,AD$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AD$7&gt;=$F38,AD$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AE38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AE$7&gt;=$F38,AE$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AE$7&gt;=$F38,AE$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AF38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AF$7&gt;=$F38,AF$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AF$7&gt;=$F38,AF$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AG38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AG$7&gt;=$F38,AG$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AG$7&gt;=$F38,AG$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AH38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AH$7&gt;=$F38,AH$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AH$7&gt;=$F38,AH$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AI38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AI$7&gt;=$F38,AI$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AI$7&gt;=$F38,AI$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AJ$7&gt;=$F38,AJ$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AJ$7&gt;=$F38,AJ$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AK38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AK$7&gt;=$F38,AK$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AK$7&gt;=$F38,AK$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AL38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AL$7&gt;=$F38,AL$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AL$7&gt;=$F38,AL$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AM38" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C38="Goal",AM$7&gt;=$F38,AM$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AM$7&gt;=$F38,AM$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AN38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AN$7&gt;=$F38,AN$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AN$7&gt;=$F38,AN$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AO38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AO$7&gt;=$F38,AO$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AO$7&gt;=$F38,AO$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AP38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AP$7&gt;=$F38,AP$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AP$7&gt;=$F38,AP$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AQ$7&gt;=$F38,AQ$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AQ$7&gt;=$F38,AQ$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AR38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AR$7&gt;=$F38,AR$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AR$7&gt;=$F38,AR$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AS38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AS$7&gt;=$F38,AS$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AS$7&gt;=$F38,AS$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AT38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AT$7&gt;=$F38,AT$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AT$7&gt;=$F38,AT$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AU38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AU$7&gt;=$F38,AU$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AU$7&gt;=$F38,AU$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AV38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AV$7&gt;=$F38,AV$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AV$7&gt;=$F38,AV$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AW38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AW$7&gt;=$F38,AW$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AW$7&gt;=$F38,AW$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AX38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AX$7&gt;=$F38,AX$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AX$7&gt;=$F38,AX$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AY38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AY$7&gt;=$F38,AY$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AY$7&gt;=$F38,AY$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",AZ$7&gt;=$F38,AZ$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",AZ$7&gt;=$F38,AZ$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BA38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",BA$7&gt;=$F38,BA$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BA$7&gt;=$F38,BA$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BB38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",BB$7&gt;=$F38,BB$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BB$7&gt;=$F38,BB$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BC38" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C38="Goal",BC$7&gt;=$F38,BC$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BC$7&gt;=$F38,BC$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BD38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BD$7&gt;=$F38,BD$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BD$7&gt;=$F38,BD$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BE38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BE$7&gt;=$F38,BE$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BE$7&gt;=$F38,BE$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BF38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BF$7&gt;=$F38,BF$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BF$7&gt;=$F38,BF$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BG38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BG$7&gt;=$F38,BG$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BG$7&gt;=$F38,BG$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BH38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BH$7&gt;=$F38,BH$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BH$7&gt;=$F38,BH$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BI38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BI$7&gt;=$F38,BI$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BI$7&gt;=$F38,BI$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BJ$7&gt;=$F38,BJ$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BJ$7&gt;=$F38,BJ$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BK38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BK$7&gt;=$F38,BK$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BK$7&gt;=$F38,BK$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BL38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BL$7&gt;=$F38,BL$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BL$7&gt;=$F38,BL$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BM38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BM$7&gt;=$F38,BM$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BM$7&gt;=$F38,BM$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BN38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BN$7&gt;=$F38,BN$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BN$7&gt;=$F38,BN$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BO38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BO$7&gt;=$F38,BO$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BO$7&gt;=$F38,BO$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BP38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BP$7&gt;=$F38,BP$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BP$7&gt;=$F38,BP$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BQ$7&gt;=$F38,BQ$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BQ$7&gt;=$F38,BQ$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BR38" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C38="Goal",BR$7&gt;=$F38,BR$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BR$7&gt;=$F38,BR$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BS38" s="17" t="str">
-        <f t="shared" ref="BS38:BU43" ca="1" si="26">IF(AND($C38="Goal",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),1,""))</f>
+        <f ca="1">IF(AND($C38="Goal",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BS$7&gt;=$F38,BS$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BT38" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C38="Goal",BT$7&gt;=$F38,BT$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BT$7&gt;=$F38,BT$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
       <c r="BU38" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C38="Goal",BU$7&gt;=$F38,BU$7&lt;=$F38+$G38-1),2,IF(AND($C38="Milestone",BU$7&gt;=$F38,BU$7&lt;=$F38+$G38-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="71"/>
       <c r="B39" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" s="62" t="s">
         <v>29</v>
@@ -8495,560 +8633,560 @@
       </c>
       <c r="F39" s="64">
         <f>F31+G31</f>
-        <v>45388.5</v>
+        <v>45388</v>
       </c>
       <c r="G39" s="65">
         <v>2</v>
       </c>
       <c r="H39" s="19"/>
       <c r="I39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",I$7&gt;=$F39,I$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",I$7&gt;=$F39,I$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="J39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",J$7&gt;=$F39,J$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",J$7&gt;=$F39,J$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="K39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",K$7&gt;=$F39,K$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",K$7&gt;=$F39,K$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="L39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",L$7&gt;=$F39,L$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",L$7&gt;=$F39,L$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="M39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",M$7&gt;=$F39,M$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",M$7&gt;=$F39,M$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="N39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",N$7&gt;=$F39,N$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",N$7&gt;=$F39,N$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="O39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",O$7&gt;=$F39,O$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",O$7&gt;=$F39,O$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="P39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",P$7&gt;=$F39,P$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",P$7&gt;=$F39,P$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="Q39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",Q$7&gt;=$F39,Q$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",Q$7&gt;=$F39,Q$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="R39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",R$7&gt;=$F39,R$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",R$7&gt;=$F39,R$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="S39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",S$7&gt;=$F39,S$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",S$7&gt;=$F39,S$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="T39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",T$7&gt;=$F39,T$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",T$7&gt;=$F39,T$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="U39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",U$7&gt;=$F39,U$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",U$7&gt;=$F39,U$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="V39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",V$7&gt;=$F39,V$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",V$7&gt;=$F39,V$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="W39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",W$7&gt;=$F39,W$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",W$7&gt;=$F39,W$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="X39" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C39="Goal",X$7&gt;=$F39,X$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",X$7&gt;=$F39,X$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="Y39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",Y$7&gt;=$F39,Y$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",Y$7&gt;=$F39,Y$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="Z39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",Z$7&gt;=$F39,Z$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",Z$7&gt;=$F39,Z$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AA39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AA$7&gt;=$F39,AA$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AA$7&gt;=$F39,AA$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AB39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AB$7&gt;=$F39,AB$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AB$7&gt;=$F39,AB$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AC39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AC$7&gt;=$F39,AC$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AC$7&gt;=$F39,AC$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AD39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AD$7&gt;=$F39,AD$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AD$7&gt;=$F39,AD$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AE39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AE$7&gt;=$F39,AE$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AE$7&gt;=$F39,AE$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AF39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AF$7&gt;=$F39,AF$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AF$7&gt;=$F39,AF$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AG39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AG$7&gt;=$F39,AG$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AG$7&gt;=$F39,AG$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AH39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AH$7&gt;=$F39,AH$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AH$7&gt;=$F39,AH$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AI39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AI$7&gt;=$F39,AI$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AI$7&gt;=$F39,AI$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AJ$7&gt;=$F39,AJ$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AJ$7&gt;=$F39,AJ$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AK39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AK$7&gt;=$F39,AK$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AK$7&gt;=$F39,AK$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AL39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AL$7&gt;=$F39,AL$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AL$7&gt;=$F39,AL$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AM39" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C39="Goal",AM$7&gt;=$F39,AM$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AM$7&gt;=$F39,AM$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AN39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AN$7&gt;=$F39,AN$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AN$7&gt;=$F39,AN$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AO39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AO$7&gt;=$F39,AO$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AO$7&gt;=$F39,AO$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AP39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AP$7&gt;=$F39,AP$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AP$7&gt;=$F39,AP$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AQ$7&gt;=$F39,AQ$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AQ$7&gt;=$F39,AQ$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AR39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AR$7&gt;=$F39,AR$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AR$7&gt;=$F39,AR$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AS39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AS$7&gt;=$F39,AS$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AS$7&gt;=$F39,AS$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AT39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AT$7&gt;=$F39,AT$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AT$7&gt;=$F39,AT$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AU39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AU$7&gt;=$F39,AU$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AU$7&gt;=$F39,AU$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AV39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AV$7&gt;=$F39,AV$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AV$7&gt;=$F39,AV$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AW39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AW$7&gt;=$F39,AW$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AW$7&gt;=$F39,AW$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AX39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AX$7&gt;=$F39,AX$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AX$7&gt;=$F39,AX$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AY39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AY$7&gt;=$F39,AY$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AY$7&gt;=$F39,AY$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",AZ$7&gt;=$F39,AZ$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",AZ$7&gt;=$F39,AZ$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BA39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",BA$7&gt;=$F39,BA$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BA$7&gt;=$F39,BA$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BB39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",BB$7&gt;=$F39,BB$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BB$7&gt;=$F39,BB$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BC39" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C39="Goal",BC$7&gt;=$F39,BC$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BC$7&gt;=$F39,BC$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BD39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BD$7&gt;=$F39,BD$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BD$7&gt;=$F39,BD$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BE39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BE$7&gt;=$F39,BE$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BE$7&gt;=$F39,BE$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BF39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BF$7&gt;=$F39,BF$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BF$7&gt;=$F39,BF$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BG39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BG$7&gt;=$F39,BG$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BG$7&gt;=$F39,BG$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BH39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BH$7&gt;=$F39,BH$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BH$7&gt;=$F39,BH$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BI39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BI$7&gt;=$F39,BI$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BI$7&gt;=$F39,BI$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BJ$7&gt;=$F39,BJ$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BJ$7&gt;=$F39,BJ$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BK39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BK$7&gt;=$F39,BK$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BK$7&gt;=$F39,BK$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BL39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BL$7&gt;=$F39,BL$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BL$7&gt;=$F39,BL$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BM39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BM$7&gt;=$F39,BM$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BM$7&gt;=$F39,BM$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BN39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BN$7&gt;=$F39,BN$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BN$7&gt;=$F39,BN$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BO39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BO$7&gt;=$F39,BO$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BO$7&gt;=$F39,BO$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BP39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BP$7&gt;=$F39,BP$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BP$7&gt;=$F39,BP$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BQ$7&gt;=$F39,BQ$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BQ$7&gt;=$F39,BQ$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BR39" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C39="Goal",BR$7&gt;=$F39,BR$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BR$7&gt;=$F39,BR$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BS39" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C39="Goal",BS$7&gt;=$F39,BS$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BS$7&gt;=$F39,BS$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BT39" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C39="Goal",BT$7&gt;=$F39,BT$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BT$7&gt;=$F39,BT$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
       <c r="BU39" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C39="Goal",BU$7&gt;=$F39,BU$7&lt;=$F39+$G39-1),2,IF(AND($C39="Milestone",BU$7&gt;=$F39,BU$7&lt;=$F39+$G39-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="71"/>
       <c r="B40" s="66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="62" t="s">
         <v>29</v>
       </c>
       <c r="D40" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E40" s="63">
         <v>0</v>
       </c>
       <c r="F40" s="64">
         <f>F39+G39</f>
-        <v>45390.5</v>
+        <v>45390</v>
       </c>
       <c r="G40" s="65">
         <v>2</v>
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",I$7&gt;=$F40,I$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",I$7&gt;=$F40,I$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="J40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",J$7&gt;=$F40,J$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",J$7&gt;=$F40,J$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="K40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",K$7&gt;=$F40,K$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",K$7&gt;=$F40,K$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="L40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",L$7&gt;=$F40,L$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",L$7&gt;=$F40,L$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="M40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",M$7&gt;=$F40,M$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",M$7&gt;=$F40,M$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="N40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",N$7&gt;=$F40,N$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",N$7&gt;=$F40,N$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="O40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",O$7&gt;=$F40,O$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",O$7&gt;=$F40,O$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="P40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",P$7&gt;=$F40,P$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",P$7&gt;=$F40,P$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="Q40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",Q$7&gt;=$F40,Q$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",Q$7&gt;=$F40,Q$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="R40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",R$7&gt;=$F40,R$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",R$7&gt;=$F40,R$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="S40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",S$7&gt;=$F40,S$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",S$7&gt;=$F40,S$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="T40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",T$7&gt;=$F40,T$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",T$7&gt;=$F40,T$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="U40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",U$7&gt;=$F40,U$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",U$7&gt;=$F40,U$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="V40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",V$7&gt;=$F40,V$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",V$7&gt;=$F40,V$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="W40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",W$7&gt;=$F40,W$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",W$7&gt;=$F40,W$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="X40" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C40="Goal",X$7&gt;=$F40,X$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",X$7&gt;=$F40,X$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="Y40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",Y$7&gt;=$F40,Y$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",Y$7&gt;=$F40,Y$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="Z40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",Z$7&gt;=$F40,Z$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",Z$7&gt;=$F40,Z$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AA40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AA$7&gt;=$F40,AA$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AA$7&gt;=$F40,AA$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AB40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AB$7&gt;=$F40,AB$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AB$7&gt;=$F40,AB$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AC40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AC$7&gt;=$F40,AC$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AC$7&gt;=$F40,AC$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AD40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AD$7&gt;=$F40,AD$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AD$7&gt;=$F40,AD$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AE40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AE$7&gt;=$F40,AE$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AE$7&gt;=$F40,AE$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AF40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AF$7&gt;=$F40,AF$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AF$7&gt;=$F40,AF$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AG40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AG$7&gt;=$F40,AG$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AG$7&gt;=$F40,AG$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AH40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AH$7&gt;=$F40,AH$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AH$7&gt;=$F40,AH$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AI40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AI$7&gt;=$F40,AI$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AI$7&gt;=$F40,AI$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AJ$7&gt;=$F40,AJ$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AJ$7&gt;=$F40,AJ$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AK40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AK$7&gt;=$F40,AK$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AK$7&gt;=$F40,AK$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AL40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AL$7&gt;=$F40,AL$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AL$7&gt;=$F40,AL$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AM40" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C40="Goal",AM$7&gt;=$F40,AM$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AM$7&gt;=$F40,AM$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AN40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AN$7&gt;=$F40,AN$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AN$7&gt;=$F40,AN$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AO40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AO$7&gt;=$F40,AO$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AO$7&gt;=$F40,AO$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AP40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AP$7&gt;=$F40,AP$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AP$7&gt;=$F40,AP$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AQ$7&gt;=$F40,AQ$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AQ$7&gt;=$F40,AQ$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AR40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AR$7&gt;=$F40,AR$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AR$7&gt;=$F40,AR$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AS40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AS$7&gt;=$F40,AS$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AS$7&gt;=$F40,AS$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AT40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AT$7&gt;=$F40,AT$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AT$7&gt;=$F40,AT$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AU40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AU$7&gt;=$F40,AU$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AU$7&gt;=$F40,AU$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AV40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AV$7&gt;=$F40,AV$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AV$7&gt;=$F40,AV$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AW40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AW$7&gt;=$F40,AW$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AW$7&gt;=$F40,AW$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AX40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AX$7&gt;=$F40,AX$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AX$7&gt;=$F40,AX$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AY40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AY$7&gt;=$F40,AY$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AY$7&gt;=$F40,AY$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",AZ$7&gt;=$F40,AZ$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",AZ$7&gt;=$F40,AZ$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BA40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",BA$7&gt;=$F40,BA$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BA$7&gt;=$F40,BA$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BB40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",BB$7&gt;=$F40,BB$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BB$7&gt;=$F40,BB$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BC40" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C40="Goal",BC$7&gt;=$F40,BC$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BC$7&gt;=$F40,BC$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BD40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BD$7&gt;=$F40,BD$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BD$7&gt;=$F40,BD$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BE40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BE$7&gt;=$F40,BE$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BE$7&gt;=$F40,BE$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BF40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BF$7&gt;=$F40,BF$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BF$7&gt;=$F40,BF$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BG40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BG$7&gt;=$F40,BG$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BG$7&gt;=$F40,BG$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BH40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BH$7&gt;=$F40,BH$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BH$7&gt;=$F40,BH$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BI40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BI$7&gt;=$F40,BI$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BI$7&gt;=$F40,BI$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BJ$7&gt;=$F40,BJ$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BJ$7&gt;=$F40,BJ$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BK40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BK$7&gt;=$F40,BK$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BK$7&gt;=$F40,BK$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BL40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BL$7&gt;=$F40,BL$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BL$7&gt;=$F40,BL$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BM40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BM$7&gt;=$F40,BM$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BM$7&gt;=$F40,BM$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BN40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BN$7&gt;=$F40,BN$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BN$7&gt;=$F40,BN$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BO40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BO$7&gt;=$F40,BO$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BO$7&gt;=$F40,BO$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BP40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BP$7&gt;=$F40,BP$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BP$7&gt;=$F40,BP$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BQ$7&gt;=$F40,BQ$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BQ$7&gt;=$F40,BQ$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BR40" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C40="Goal",BR$7&gt;=$F40,BR$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BR$7&gt;=$F40,BR$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BS40" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C40="Goal",BS$7&gt;=$F40,BS$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BS$7&gt;=$F40,BS$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BT40" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C40="Goal",BT$7&gt;=$F40,BT$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BT$7&gt;=$F40,BT$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
       <c r="BU40" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C40="Goal",BU$7&gt;=$F40,BU$7&lt;=$F40+$G40-1),2,IF(AND($C40="Milestone",BU$7&gt;=$F40,BU$7&lt;=$F40+$G40-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="71"/>
       <c r="B41" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="62" t="s">
         <v>29</v>
@@ -9061,277 +9199,277 @@
       </c>
       <c r="F41" s="64">
         <f>F39+G39</f>
-        <v>45390.5</v>
+        <v>45390</v>
       </c>
       <c r="G41" s="65">
         <v>3</v>
       </c>
       <c r="H41" s="19"/>
       <c r="I41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",I$7&gt;=$F41,I$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",I$7&gt;=$F41,I$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="J41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",J$7&gt;=$F41,J$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",J$7&gt;=$F41,J$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="K41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",K$7&gt;=$F41,K$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",K$7&gt;=$F41,K$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="L41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",L$7&gt;=$F41,L$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",L$7&gt;=$F41,L$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="M41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",M$7&gt;=$F41,M$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",M$7&gt;=$F41,M$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="N41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",N$7&gt;=$F41,N$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",N$7&gt;=$F41,N$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="O41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",O$7&gt;=$F41,O$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",O$7&gt;=$F41,O$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="P41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",P$7&gt;=$F41,P$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",P$7&gt;=$F41,P$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="Q41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",Q$7&gt;=$F41,Q$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",Q$7&gt;=$F41,Q$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="R41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",R$7&gt;=$F41,R$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",R$7&gt;=$F41,R$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="S41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",S$7&gt;=$F41,S$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",S$7&gt;=$F41,S$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="T41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",T$7&gt;=$F41,T$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",T$7&gt;=$F41,T$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="U41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",U$7&gt;=$F41,U$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",U$7&gt;=$F41,U$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="V41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",V$7&gt;=$F41,V$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",V$7&gt;=$F41,V$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="W41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",W$7&gt;=$F41,W$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",W$7&gt;=$F41,W$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="X41" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C41="Goal",X$7&gt;=$F41,X$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",X$7&gt;=$F41,X$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="Y41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",Y$7&gt;=$F41,Y$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",Y$7&gt;=$F41,Y$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="Z41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",Z$7&gt;=$F41,Z$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",Z$7&gt;=$F41,Z$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AA41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AA$7&gt;=$F41,AA$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AA$7&gt;=$F41,AA$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AB41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AB$7&gt;=$F41,AB$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AB$7&gt;=$F41,AB$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AC41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AC$7&gt;=$F41,AC$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AC$7&gt;=$F41,AC$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AD41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AD$7&gt;=$F41,AD$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AD$7&gt;=$F41,AD$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AE41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AE$7&gt;=$F41,AE$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AE$7&gt;=$F41,AE$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AF41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AF$7&gt;=$F41,AF$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AF$7&gt;=$F41,AF$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AG41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AG$7&gt;=$F41,AG$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AG$7&gt;=$F41,AG$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AH41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AH$7&gt;=$F41,AH$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AH$7&gt;=$F41,AH$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AI41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AI$7&gt;=$F41,AI$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AI$7&gt;=$F41,AI$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AJ$7&gt;=$F41,AJ$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AJ$7&gt;=$F41,AJ$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AK41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AK$7&gt;=$F41,AK$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AK$7&gt;=$F41,AK$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AL41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AL$7&gt;=$F41,AL$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AL$7&gt;=$F41,AL$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AM41" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C41="Goal",AM$7&gt;=$F41,AM$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AM$7&gt;=$F41,AM$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AN41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AN$7&gt;=$F41,AN$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AN$7&gt;=$F41,AN$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AO41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AO$7&gt;=$F41,AO$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AO$7&gt;=$F41,AO$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AP41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AP$7&gt;=$F41,AP$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AP$7&gt;=$F41,AP$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AQ$7&gt;=$F41,AQ$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AQ$7&gt;=$F41,AQ$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AR41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AR$7&gt;=$F41,AR$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AR$7&gt;=$F41,AR$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AS41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AS$7&gt;=$F41,AS$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AS$7&gt;=$F41,AS$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AT41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AT$7&gt;=$F41,AT$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AT$7&gt;=$F41,AT$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AU41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AU$7&gt;=$F41,AU$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AU$7&gt;=$F41,AU$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AV41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AV$7&gt;=$F41,AV$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AV$7&gt;=$F41,AV$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AW41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AW$7&gt;=$F41,AW$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AW$7&gt;=$F41,AW$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AX41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AX$7&gt;=$F41,AX$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AX$7&gt;=$F41,AX$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AY41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AY$7&gt;=$F41,AY$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AY$7&gt;=$F41,AY$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",AZ$7&gt;=$F41,AZ$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",AZ$7&gt;=$F41,AZ$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BA41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",BA$7&gt;=$F41,BA$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BA$7&gt;=$F41,BA$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BB41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",BB$7&gt;=$F41,BB$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BB$7&gt;=$F41,BB$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BC41" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C41="Goal",BC$7&gt;=$F41,BC$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BC$7&gt;=$F41,BC$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BD41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BD$7&gt;=$F41,BD$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BD$7&gt;=$F41,BD$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BE41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BE$7&gt;=$F41,BE$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BE$7&gt;=$F41,BE$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BF41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BF$7&gt;=$F41,BF$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BF$7&gt;=$F41,BF$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BG41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BG$7&gt;=$F41,BG$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BG$7&gt;=$F41,BG$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BH41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BH$7&gt;=$F41,BH$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BH$7&gt;=$F41,BH$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BI41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BI$7&gt;=$F41,BI$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BI$7&gt;=$F41,BI$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BJ$7&gt;=$F41,BJ$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BJ$7&gt;=$F41,BJ$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BK41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BK$7&gt;=$F41,BK$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BK$7&gt;=$F41,BK$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BL41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BL$7&gt;=$F41,BL$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BL$7&gt;=$F41,BL$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BM41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BM$7&gt;=$F41,BM$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BM$7&gt;=$F41,BM$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BN41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BN$7&gt;=$F41,BN$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BN$7&gt;=$F41,BN$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BO41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BO$7&gt;=$F41,BO$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BO$7&gt;=$F41,BO$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BP41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BP$7&gt;=$F41,BP$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BP$7&gt;=$F41,BP$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BQ$7&gt;=$F41,BQ$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BQ$7&gt;=$F41,BQ$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BR41" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C41="Goal",BR$7&gt;=$F41,BR$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BR$7&gt;=$F41,BR$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BS41" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C41="Goal",BS$7&gt;=$F41,BS$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BS$7&gt;=$F41,BS$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BT41" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C41="Goal",BT$7&gt;=$F41,BT$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BT$7&gt;=$F41,BT$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
       <c r="BU41" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C41="Goal",BU$7&gt;=$F41,BU$7&lt;=$F41+$G41-1),2,IF(AND($C41="Milestone",BU$7&gt;=$F41,BU$7&lt;=$F41+$G41-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="71"/>
       <c r="B42" s="66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" s="62" t="s">
         <v>29</v>
@@ -9344,277 +9482,277 @@
       </c>
       <c r="F42" s="64">
         <f>F41+G41</f>
-        <v>45393.5</v>
+        <v>45393</v>
       </c>
       <c r="G42" s="65">
         <v>5</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",I$7&gt;=$F42,I$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",I$7&gt;=$F42,I$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="J42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",J$7&gt;=$F42,J$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",J$7&gt;=$F42,J$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="K42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",K$7&gt;=$F42,K$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",K$7&gt;=$F42,K$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="L42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",L$7&gt;=$F42,L$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",L$7&gt;=$F42,L$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="M42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",M$7&gt;=$F42,M$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",M$7&gt;=$F42,M$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="N42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",N$7&gt;=$F42,N$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",N$7&gt;=$F42,N$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="O42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",O$7&gt;=$F42,O$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",O$7&gt;=$F42,O$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="P42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",P$7&gt;=$F42,P$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",P$7&gt;=$F42,P$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="Q42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",Q$7&gt;=$F42,Q$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",Q$7&gt;=$F42,Q$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="R42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",R$7&gt;=$F42,R$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",R$7&gt;=$F42,R$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="S42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",S$7&gt;=$F42,S$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",S$7&gt;=$F42,S$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="T42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",T$7&gt;=$F42,T$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",T$7&gt;=$F42,T$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="U42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",U$7&gt;=$F42,U$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",U$7&gt;=$F42,U$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="V42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",V$7&gt;=$F42,V$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",V$7&gt;=$F42,V$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="W42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",W$7&gt;=$F42,W$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",W$7&gt;=$F42,W$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="X42" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C42="Goal",X$7&gt;=$F42,X$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",X$7&gt;=$F42,X$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="Y42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",Y$7&gt;=$F42,Y$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",Y$7&gt;=$F42,Y$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="Z42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",Z$7&gt;=$F42,Z$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",Z$7&gt;=$F42,Z$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AA42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AA$7&gt;=$F42,AA$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AA$7&gt;=$F42,AA$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AB42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AB$7&gt;=$F42,AB$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AB$7&gt;=$F42,AB$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AC42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AC$7&gt;=$F42,AC$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AC$7&gt;=$F42,AC$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AD42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AD$7&gt;=$F42,AD$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AD$7&gt;=$F42,AD$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AE42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AE$7&gt;=$F42,AE$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AE$7&gt;=$F42,AE$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AF42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AF$7&gt;=$F42,AF$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AF$7&gt;=$F42,AF$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AG42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AG$7&gt;=$F42,AG$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AG$7&gt;=$F42,AG$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AH42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AH$7&gt;=$F42,AH$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AH$7&gt;=$F42,AH$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AI42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AI$7&gt;=$F42,AI$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AI$7&gt;=$F42,AI$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AJ$7&gt;=$F42,AJ$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AJ$7&gt;=$F42,AJ$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AK42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AK$7&gt;=$F42,AK$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AK$7&gt;=$F42,AK$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AL42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AL$7&gt;=$F42,AL$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AL$7&gt;=$F42,AL$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AM42" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C42="Goal",AM$7&gt;=$F42,AM$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AM$7&gt;=$F42,AM$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AN42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AN$7&gt;=$F42,AN$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AN$7&gt;=$F42,AN$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AO42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AO$7&gt;=$F42,AO$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AO$7&gt;=$F42,AO$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AP42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AP$7&gt;=$F42,AP$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AP$7&gt;=$F42,AP$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AQ$7&gt;=$F42,AQ$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AQ$7&gt;=$F42,AQ$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AR42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AR$7&gt;=$F42,AR$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AR$7&gt;=$F42,AR$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AS42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AS$7&gt;=$F42,AS$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AS$7&gt;=$F42,AS$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AT42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AT$7&gt;=$F42,AT$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AT$7&gt;=$F42,AT$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AU42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AU$7&gt;=$F42,AU$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AU$7&gt;=$F42,AU$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AV42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AV$7&gt;=$F42,AV$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AV$7&gt;=$F42,AV$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AW42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AW$7&gt;=$F42,AW$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AW$7&gt;=$F42,AW$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AX42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AX$7&gt;=$F42,AX$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AX$7&gt;=$F42,AX$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AY42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AY$7&gt;=$F42,AY$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AY$7&gt;=$F42,AY$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",AZ$7&gt;=$F42,AZ$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",AZ$7&gt;=$F42,AZ$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BA42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",BA$7&gt;=$F42,BA$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BA$7&gt;=$F42,BA$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BB42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",BB$7&gt;=$F42,BB$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BB$7&gt;=$F42,BB$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BC42" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C42="Goal",BC$7&gt;=$F42,BC$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BC$7&gt;=$F42,BC$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BD42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BD$7&gt;=$F42,BD$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BD$7&gt;=$F42,BD$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BE42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BE$7&gt;=$F42,BE$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BE$7&gt;=$F42,BE$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BF42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BF$7&gt;=$F42,BF$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BF$7&gt;=$F42,BF$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BG42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BG$7&gt;=$F42,BG$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BG$7&gt;=$F42,BG$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BH42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BH$7&gt;=$F42,BH$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BH$7&gt;=$F42,BH$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BI42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BI$7&gt;=$F42,BI$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BI$7&gt;=$F42,BI$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BJ$7&gt;=$F42,BJ$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BJ$7&gt;=$F42,BJ$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BK42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BK$7&gt;=$F42,BK$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BK$7&gt;=$F42,BK$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BL42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BL$7&gt;=$F42,BL$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BL$7&gt;=$F42,BL$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BM42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BM$7&gt;=$F42,BM$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BM$7&gt;=$F42,BM$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BN42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BN$7&gt;=$F42,BN$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BN$7&gt;=$F42,BN$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BO42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BO$7&gt;=$F42,BO$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BO$7&gt;=$F42,BO$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BP42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BP$7&gt;=$F42,BP$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BP$7&gt;=$F42,BP$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BQ$7&gt;=$F42,BQ$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BQ$7&gt;=$F42,BQ$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BR42" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C42="Goal",BR$7&gt;=$F42,BR$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BR$7&gt;=$F42,BR$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BS42" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C42="Goal",BS$7&gt;=$F42,BS$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BS$7&gt;=$F42,BS$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BT42" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C42="Goal",BT$7&gt;=$F42,BT$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BT$7&gt;=$F42,BT$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="BU42" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C42="Goal",BU$7&gt;=$F42,BU$7&lt;=$F42+$G42-1),2,IF(AND($C42="Milestone",BU$7&gt;=$F42,BU$7&lt;=$F42+$G42-1),1,""))</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:73" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="71"/>
       <c r="B43" s="66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="62" t="s">
         <v>29</v>
@@ -9627,270 +9765,270 @@
       </c>
       <c r="F43" s="64">
         <f>F42+G42-1</f>
-        <v>45397.5</v>
+        <v>45397</v>
       </c>
       <c r="G43" s="65">
         <v>15</v>
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",I$7&gt;=$F43,I$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",I$7&gt;=$F43,I$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="J43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",J$7&gt;=$F43,J$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",J$7&gt;=$F43,J$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="K43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",K$7&gt;=$F43,K$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",K$7&gt;=$F43,K$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="L43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",L$7&gt;=$F43,L$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",L$7&gt;=$F43,L$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="M43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",M$7&gt;=$F43,M$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",M$7&gt;=$F43,M$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="N43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",N$7&gt;=$F43,N$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",N$7&gt;=$F43,N$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="O43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",O$7&gt;=$F43,O$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",O$7&gt;=$F43,O$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="P43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",P$7&gt;=$F43,P$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",P$7&gt;=$F43,P$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="Q43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",Q$7&gt;=$F43,Q$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",Q$7&gt;=$F43,Q$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="R43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",R$7&gt;=$F43,R$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",R$7&gt;=$F43,R$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="S43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",S$7&gt;=$F43,S$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",S$7&gt;=$F43,S$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="T43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",T$7&gt;=$F43,T$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",T$7&gt;=$F43,T$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="U43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",U$7&gt;=$F43,U$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",U$7&gt;=$F43,U$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="V43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",V$7&gt;=$F43,V$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",V$7&gt;=$F43,V$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="W43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",W$7&gt;=$F43,W$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",W$7&gt;=$F43,W$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="X43" s="17" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f ca="1">IF(AND($C43="Goal",X$7&gt;=$F43,X$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",X$7&gt;=$F43,X$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="Y43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",Y$7&gt;=$F43,Y$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",Y$7&gt;=$F43,Y$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="Z43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",Z$7&gt;=$F43,Z$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",Z$7&gt;=$F43,Z$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AA43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AA$7&gt;=$F43,AA$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AA$7&gt;=$F43,AA$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AB43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AB$7&gt;=$F43,AB$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AB$7&gt;=$F43,AB$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AC43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AC$7&gt;=$F43,AC$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AC$7&gt;=$F43,AC$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AD43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AD$7&gt;=$F43,AD$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AD$7&gt;=$F43,AD$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AE43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AE$7&gt;=$F43,AE$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AE$7&gt;=$F43,AE$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AF43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AF$7&gt;=$F43,AF$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AF$7&gt;=$F43,AF$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AG43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AG$7&gt;=$F43,AG$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AG$7&gt;=$F43,AG$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AH43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AH$7&gt;=$F43,AH$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AH$7&gt;=$F43,AH$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AI43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AI$7&gt;=$F43,AI$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AI$7&gt;=$F43,AI$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AJ43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AJ$7&gt;=$F43,AJ$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AJ$7&gt;=$F43,AJ$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AK43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AK$7&gt;=$F43,AK$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AK$7&gt;=$F43,AK$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AL43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AL$7&gt;=$F43,AL$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AL$7&gt;=$F43,AL$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AM43" s="17" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f ca="1">IF(AND($C43="Goal",AM$7&gt;=$F43,AM$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AM$7&gt;=$F43,AM$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AN43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AN$7&gt;=$F43,AN$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AN$7&gt;=$F43,AN$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AO43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AO$7&gt;=$F43,AO$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AO$7&gt;=$F43,AO$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AP43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AP$7&gt;=$F43,AP$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AP$7&gt;=$F43,AP$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AQ$7&gt;=$F43,AQ$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AQ$7&gt;=$F43,AQ$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AR43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AR$7&gt;=$F43,AR$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AR$7&gt;=$F43,AR$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AS43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AS$7&gt;=$F43,AS$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AS$7&gt;=$F43,AS$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AT43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AT$7&gt;=$F43,AT$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AT$7&gt;=$F43,AT$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AU43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AU$7&gt;=$F43,AU$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AU$7&gt;=$F43,AU$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AV43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AV$7&gt;=$F43,AV$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AV$7&gt;=$F43,AV$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AW43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AW$7&gt;=$F43,AW$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AW$7&gt;=$F43,AW$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AX43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AX$7&gt;=$F43,AX$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AX$7&gt;=$F43,AX$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AY43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AY$7&gt;=$F43,AY$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AY$7&gt;=$F43,AY$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="AZ43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",AZ$7&gt;=$F43,AZ$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",AZ$7&gt;=$F43,AZ$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BA43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",BA$7&gt;=$F43,BA$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BA$7&gt;=$F43,BA$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BB43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",BB$7&gt;=$F43,BB$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BB$7&gt;=$F43,BB$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BC43" s="17" t="str">
-        <f t="shared" ca="1" si="22"/>
+        <f ca="1">IF(AND($C43="Goal",BC$7&gt;=$F43,BC$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BC$7&gt;=$F43,BC$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BD43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BD$7&gt;=$F43,BD$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BD$7&gt;=$F43,BD$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BE43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BE$7&gt;=$F43,BE$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BE$7&gt;=$F43,BE$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BF43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BF$7&gt;=$F43,BF$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BF$7&gt;=$F43,BF$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BG43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BG$7&gt;=$F43,BG$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BG$7&gt;=$F43,BG$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BH43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BH$7&gt;=$F43,BH$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BH$7&gt;=$F43,BH$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BI43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BI$7&gt;=$F43,BI$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BI$7&gt;=$F43,BI$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BJ43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BJ$7&gt;=$F43,BJ$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BJ$7&gt;=$F43,BJ$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BK43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BK$7&gt;=$F43,BK$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BK$7&gt;=$F43,BK$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BL43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BL$7&gt;=$F43,BL$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BL$7&gt;=$F43,BL$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BM43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BM$7&gt;=$F43,BM$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BM$7&gt;=$F43,BM$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BN43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BN$7&gt;=$F43,BN$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BN$7&gt;=$F43,BN$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BO43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BO$7&gt;=$F43,BO$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BO$7&gt;=$F43,BO$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BP43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BP$7&gt;=$F43,BP$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BP$7&gt;=$F43,BP$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BQ43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BQ$7&gt;=$F43,BQ$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BQ$7&gt;=$F43,BQ$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BR43" s="17" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f ca="1">IF(AND($C43="Goal",BR$7&gt;=$F43,BR$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BR$7&gt;=$F43,BR$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BS43" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C43="Goal",BS$7&gt;=$F43,BS$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BS$7&gt;=$F43,BS$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BT43" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C43="Goal",BT$7&gt;=$F43,BT$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BT$7&gt;=$F43,BT$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
       <c r="BU43" s="17" t="str">
-        <f t="shared" ca="1" si="26"/>
+        <f ca="1">IF(AND($C43="Goal",BU$7&gt;=$F43,BU$7&lt;=$F43+$G43-1),2,IF(AND($C43="Milestone",BU$7&gt;=$F43,BU$7&lt;=$F43+$G43-1),1,""))</f>
         <v/>
       </c>
     </row>
@@ -9925,52 +10063,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BT43">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BU6">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BU43">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+  <conditionalFormatting sqref="I10:BU31">
+    <cfRule type="expression" dxfId="16" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="8" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="9" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BU6">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU7:BU43">
-    <cfRule type="expression" dxfId="0" priority="49">
+    <cfRule type="expression" dxfId="10" priority="49">
       <formula>AND(TODAY()&gt;=BU$7,TODAY()&lt;#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I33:BU43">
+    <cfRule type="expression" dxfId="9" priority="126" stopIfTrue="1">
+      <formula>AND($C33="Low Risk",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="127" stopIfTrue="1">
+      <formula>AND($C33="High Risk",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="128" stopIfTrue="1">
+      <formula>AND($C33="On Track",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="129" stopIfTrue="1">
+      <formula>AND($C33="Med Risk",I$7&gt;=$F33,I$7&lt;=$F33+$G33-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="130" stopIfTrue="1">
+      <formula>AND(LEN($C33)=0,I$7&gt;=$F33,I$7&lt;=$F33+$G33-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32:BU32">
+    <cfRule type="expression" dxfId="4" priority="132" stopIfTrue="1">
+      <formula>AND($C32="Low Risk",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="133" stopIfTrue="1">
+      <formula>AND($C32="High Risk",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="134" stopIfTrue="1">
+      <formula>AND($C32="On Track",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="135" stopIfTrue="1">
+      <formula>AND($C32="Med Risk",I$7&gt;=$F32,I$7&lt;=$F32+$G32-1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="136" stopIfTrue="1">
+      <formula>AND(LEN($C32)=0,I$7&gt;=$F32,I$7&lt;=$F32+$G32-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{662A47A0-7258-440E-8D71-BC54CBC9C651}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C43" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C31 C32:C43" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{218D9212-09C8-4DA2-9014-64503951B170}">
@@ -10027,7 +10199,45 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BU43</xm:sqref>
+          <xm:sqref>I10:BU31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="131" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I33:BU43</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="137" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I32:BU32</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -10047,15 +10257,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100329040CD17E650448811C75D3A86FB19" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4e7394bae465e0dd152f3bf3519e0af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81dd9769-e470-4c71-abd0-ce40395fb0d0" xmlns:ns3="97f26d6d-5e45-4b6a-a489-05413f707488" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f30c7f853ad86ef2df9f5f9817cec86e" ns2:_="" ns3:_="">
     <xsd:import namespace="81dd9769-e470-4c71-abd0-ce40395fb0d0"/>
@@ -10244,26 +10445,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11AAADB5-F91F-44CE-8CB6-D8472D59D975}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="81dd9769-e470-4c71-abd0-ce40395fb0d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="97f26d6d-5e45-4b6a-a489-05413f707488"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBDC3097-99E4-4C58-971A-CB9D833D16FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10282,6 +10490,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>